<commit_message>
fix import with validation optional
</commit_message>
<xml_diff>
--- a/storage/sample_excel/customers_sample_data.xlsx
+++ b/storage/sample_excel/customers_sample_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\qlbh\storage\sample_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\qlbh-dev\storage\sample_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980D4756-B504-42AC-9590-E08EE143A4C7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46703935-25C7-4EFF-91FC-AF69ABA935DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Van</t>
   </si>
@@ -46,16 +46,10 @@
     <t>Address</t>
   </si>
   <si>
-    <t>25/11/1999</t>
-  </si>
-  <si>
     <t>22 ly tu trong</t>
   </si>
   <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>25/11/1399</t>
   </si>
   <si>
     <t>Nguyen Huy</t>
@@ -110,8 +104,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +415,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +424,7 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -446,20 +442,20 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F1" t="s">
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
         <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -475,28 +471,28 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1">
+        <v>36508</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>21</v>
@@ -504,24 +500,25 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
+      <c r="E3" s="1">
+        <v>37479</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>